<commit_message>
Modified virtual toll input
</commit_message>
<xml_diff>
--- a/signal_map/signalmap_safestrip_interfaces_v5.0.xlsx
+++ b/signal_map/signalmap_safestrip_interfaces_v5.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giammarco/GoogleDriveUNITN/PHDxxx/Projects/SAFESTRIP/safestrip-mqtt-interface/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giammarco/GoogleDriveUNITN/PHDxxx/Projects/SAFESTRIP/MQTT_for_safestrip/signal_map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D49D671-9EBB-354E-9382-6FE11614B75D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079A3DB7-DA21-974A-A077-017C1D0E0FA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2480" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{FBF927E7-8919-754A-9B9B-553D825B3903}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="599">
   <si>
     <t>version:5.0</t>
   </si>
@@ -1594,15 +1594,6 @@
   </si>
   <si>
     <t>VirtualToll_input/#{RFID_ID}</t>
-  </si>
-  <si>
-    <t>strip_type</t>
-  </si>
-  <si>
-    <t>Strip Type</t>
-  </si>
-  <si>
-    <t>!!! To define</t>
   </si>
   <si>
     <t>virtual_gate_distance</t>
@@ -2649,6 +2640,51 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="34" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="44" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="29" fillId="17" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2698,51 +2734,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="29" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="42" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="43" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="44" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3062,11 +3053,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EC5FC3-03DD-9345-8521-B8CE154A93B9}">
-  <dimension ref="A1:P260"/>
+  <dimension ref="A1:P259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B210" sqref="B210"/>
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A225" sqref="A225:XFD225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="41" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3081,22 +3072,22 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="107" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="109"/>
+      <c r="B1" s="122" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="124"/>
       <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="110" t="s">
+      <c r="J1" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="111"/>
+      <c r="K1" s="126"/>
       <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
@@ -3147,13 +3138,13 @@
       <c r="K2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="112" t="s">
+      <c r="L2" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="114"/>
+      <c r="M2" s="128"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="128"/>
+      <c r="P2" s="129"/>
     </row>
     <row r="3" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -7914,19 +7905,19 @@
       <c r="P119" s="17"/>
     </row>
     <row r="120" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="115" t="s">
+      <c r="A120" s="130" t="s">
         <v>353</v>
       </c>
-      <c r="B120" s="116"/>
-      <c r="C120" s="116"/>
-      <c r="D120" s="116"/>
-      <c r="E120" s="116"/>
-      <c r="F120" s="116"/>
-      <c r="G120" s="116"/>
-      <c r="H120" s="116"/>
-      <c r="I120" s="116"/>
-      <c r="J120" s="116"/>
-      <c r="K120" s="116"/>
+      <c r="B120" s="131"/>
+      <c r="C120" s="131"/>
+      <c r="D120" s="131"/>
+      <c r="E120" s="131"/>
+      <c r="F120" s="131"/>
+      <c r="G120" s="131"/>
+      <c r="H120" s="131"/>
+      <c r="I120" s="131"/>
+      <c r="J120" s="131"/>
+      <c r="K120" s="131"/>
       <c r="L120" s="17"/>
       <c r="M120" s="17"/>
       <c r="N120" s="17"/>
@@ -8396,19 +8387,19 @@
       <c r="P133" s="17"/>
     </row>
     <row r="134" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="117" t="s">
+      <c r="A134" s="132" t="s">
         <v>381</v>
       </c>
-      <c r="B134" s="118"/>
-      <c r="C134" s="118"/>
-      <c r="D134" s="118"/>
-      <c r="E134" s="118"/>
-      <c r="F134" s="118"/>
-      <c r="G134" s="118"/>
-      <c r="H134" s="118"/>
-      <c r="I134" s="118"/>
-      <c r="J134" s="118"/>
-      <c r="K134" s="119"/>
+      <c r="B134" s="133"/>
+      <c r="C134" s="133"/>
+      <c r="D134" s="133"/>
+      <c r="E134" s="133"/>
+      <c r="F134" s="133"/>
+      <c r="G134" s="133"/>
+      <c r="H134" s="133"/>
+      <c r="I134" s="133"/>
+      <c r="J134" s="133"/>
+      <c r="K134" s="134"/>
       <c r="L134" s="17"/>
       <c r="M134" s="17"/>
       <c r="N134" s="17"/>
@@ -8420,7 +8411,7 @@
         <v>382</v>
       </c>
       <c r="B135" s="60" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C135" s="61"/>
       <c r="D135" s="62"/>
@@ -8790,19 +8781,19 @@
       </c>
     </row>
     <row r="145" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="103" t="s">
+      <c r="A145" s="118" t="s">
         <v>384</v>
       </c>
-      <c r="B145" s="104"/>
-      <c r="C145" s="104"/>
-      <c r="D145" s="104"/>
-      <c r="E145" s="104"/>
-      <c r="F145" s="104"/>
-      <c r="G145" s="104"/>
-      <c r="H145" s="104"/>
-      <c r="I145" s="104"/>
-      <c r="J145" s="104"/>
-      <c r="K145" s="104"/>
+      <c r="B145" s="119"/>
+      <c r="C145" s="119"/>
+      <c r="D145" s="119"/>
+      <c r="E145" s="119"/>
+      <c r="F145" s="119"/>
+      <c r="G145" s="119"/>
+      <c r="H145" s="119"/>
+      <c r="I145" s="119"/>
+      <c r="J145" s="119"/>
+      <c r="K145" s="119"/>
       <c r="L145" s="17"/>
       <c r="M145" s="17"/>
       <c r="N145" s="17"/>
@@ -9286,19 +9277,19 @@
       <c r="P159" s="17"/>
     </row>
     <row r="160" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A160" s="103" t="s">
+      <c r="A160" s="118" t="s">
         <v>405</v>
       </c>
-      <c r="B160" s="104"/>
-      <c r="C160" s="104"/>
-      <c r="D160" s="104"/>
-      <c r="E160" s="104"/>
-      <c r="F160" s="104"/>
-      <c r="G160" s="104"/>
-      <c r="H160" s="104"/>
-      <c r="I160" s="104"/>
-      <c r="J160" s="104"/>
-      <c r="K160" s="104"/>
+      <c r="B160" s="119"/>
+      <c r="C160" s="119"/>
+      <c r="D160" s="119"/>
+      <c r="E160" s="119"/>
+      <c r="F160" s="119"/>
+      <c r="G160" s="119"/>
+      <c r="H160" s="119"/>
+      <c r="I160" s="119"/>
+      <c r="J160" s="119"/>
+      <c r="K160" s="119"/>
       <c r="L160" s="17"/>
       <c r="M160" s="17"/>
       <c r="N160" s="17"/>
@@ -10386,19 +10377,19 @@
       <c r="P192" s="17"/>
     </row>
     <row r="193" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="105" t="s">
+      <c r="A193" s="120" t="s">
         <v>473</v>
       </c>
-      <c r="B193" s="106"/>
-      <c r="C193" s="106"/>
-      <c r="D193" s="106"/>
-      <c r="E193" s="106"/>
-      <c r="F193" s="106"/>
-      <c r="G193" s="106"/>
-      <c r="H193" s="106"/>
-      <c r="I193" s="106"/>
-      <c r="J193" s="106"/>
-      <c r="K193" s="106"/>
+      <c r="B193" s="121"/>
+      <c r="C193" s="121"/>
+      <c r="D193" s="121"/>
+      <c r="E193" s="121"/>
+      <c r="F193" s="121"/>
+      <c r="G193" s="121"/>
+      <c r="H193" s="121"/>
+      <c r="I193" s="121"/>
+      <c r="J193" s="121"/>
+      <c r="K193" s="121"/>
       <c r="L193" s="17"/>
       <c r="M193" s="17"/>
       <c r="N193" s="17"/>
@@ -11458,8 +11449,12 @@
         <v>66</v>
       </c>
       <c r="F225" s="75"/>
-      <c r="G225" s="78"/>
-      <c r="H225" s="75"/>
+      <c r="G225" s="78">
+        <v>1</v>
+      </c>
+      <c r="H225" s="75" t="s">
+        <v>70</v>
+      </c>
       <c r="I225" s="72" t="s">
         <v>29</v>
       </c>
@@ -11477,27 +11472,23 @@
     </row>
     <row r="226" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="B226" s="76"/>
+      <c r="C226" s="76" t="s">
         <v>524</v>
       </c>
-      <c r="B226" s="76" t="s">
-        <v>525</v>
-      </c>
-      <c r="C226" s="79" t="s">
-        <v>526</v>
-      </c>
       <c r="D226" s="78">
         <v>1</v>
       </c>
-      <c r="E226" s="75" t="s">
-        <v>66</v>
-      </c>
-      <c r="F226" s="75"/>
-      <c r="G226" s="78">
-        <v>1</v>
-      </c>
-      <c r="H226" s="75" t="s">
-        <v>70</v>
-      </c>
+      <c r="E226" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="F226" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="G226" s="78"/>
+      <c r="H226" s="75"/>
       <c r="I226" s="72" t="s">
         <v>29</v>
       </c>
@@ -11514,29 +11505,33 @@
       </c>
     </row>
     <row r="227" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A227" s="75" t="s">
-        <v>476</v>
-      </c>
-      <c r="B227" s="76"/>
-      <c r="C227" s="76" t="s">
-        <v>527</v>
-      </c>
-      <c r="D227" s="78">
-        <v>1</v>
-      </c>
-      <c r="E227" s="89" t="s">
+      <c r="A227" s="35" t="s">
+        <v>504</v>
+      </c>
+      <c r="B227" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C227" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D227" s="23">
+        <v>1</v>
+      </c>
+      <c r="E227" s="18" t="s">
         <v>79</v>
       </c>
       <c r="F227" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="G227" s="78"/>
-      <c r="H227" s="75"/>
-      <c r="I227" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="J227" s="73"/>
-      <c r="K227" s="74"/>
+      <c r="G227" s="23"/>
+      <c r="H227" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I227" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J227" s="20"/>
+      <c r="K227" s="21"/>
       <c r="L227" s="17" t="s">
         <v>257</v>
       </c>
@@ -11548,33 +11543,33 @@
       </c>
     </row>
     <row r="228" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A228" s="35" t="s">
-        <v>504</v>
-      </c>
-      <c r="B228" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C228" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D228" s="23">
+      <c r="A228" s="97" t="s">
+        <v>260</v>
+      </c>
+      <c r="B228" s="77" t="s">
+        <v>505</v>
+      </c>
+      <c r="C228" s="77" t="s">
+        <v>505</v>
+      </c>
+      <c r="D228" s="17">
         <v>1</v>
       </c>
       <c r="E228" s="18" t="s">
         <v>79</v>
       </c>
       <c r="F228" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="G228" s="23"/>
-      <c r="H228" s="18" t="s">
+        <v>525</v>
+      </c>
+      <c r="G228" s="17"/>
+      <c r="H228" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="I228" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="J228" s="20"/>
-      <c r="K228" s="21"/>
+      <c r="I228" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="J228" s="73"/>
+      <c r="K228" s="74"/>
       <c r="L228" s="17" t="s">
         <v>257</v>
       </c>
@@ -11586,95 +11581,95 @@
       </c>
     </row>
     <row r="229" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A229" s="97" t="s">
-        <v>260</v>
-      </c>
-      <c r="B229" s="77" t="s">
-        <v>505</v>
-      </c>
-      <c r="C229" s="77" t="s">
-        <v>505</v>
-      </c>
-      <c r="D229" s="17">
-        <v>1</v>
-      </c>
-      <c r="E229" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F229" s="37" t="s">
-        <v>528</v>
-      </c>
-      <c r="G229" s="17"/>
-      <c r="H229" s="97" t="s">
-        <v>64</v>
-      </c>
-      <c r="I229" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="J229" s="73"/>
-      <c r="K229" s="74"/>
-      <c r="L229" s="17" t="s">
-        <v>257</v>
-      </c>
+      <c r="A229" s="59" t="s">
+        <v>526</v>
+      </c>
+      <c r="B229" s="90" t="s">
+        <v>527</v>
+      </c>
+      <c r="C229" s="98"/>
+      <c r="D229" s="99"/>
+      <c r="E229" s="65"/>
+      <c r="F229" s="65"/>
+      <c r="G229" s="99"/>
+      <c r="H229" s="65"/>
+      <c r="I229" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="J229" s="65"/>
+      <c r="K229" s="66"/>
+      <c r="L229" s="17"/>
       <c r="M229" s="17"/>
       <c r="N229" s="17"/>
       <c r="O229" s="17"/>
-      <c r="P229" s="17" t="s">
-        <v>75</v>
-      </c>
+      <c r="P229" s="17"/>
     </row>
     <row r="230" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A230" s="59" t="s">
-        <v>529</v>
-      </c>
-      <c r="B230" s="90" t="s">
-        <v>530</v>
-      </c>
-      <c r="C230" s="98"/>
-      <c r="D230" s="99"/>
-      <c r="E230" s="65"/>
-      <c r="F230" s="65"/>
-      <c r="G230" s="99"/>
-      <c r="H230" s="65"/>
-      <c r="I230" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="J230" s="65"/>
-      <c r="K230" s="66"/>
+      <c r="A230" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B230" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C230" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D230" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E230" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F230" s="18"/>
+      <c r="G230" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H230" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I230" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J230" s="20"/>
+      <c r="K230" s="21"/>
       <c r="L230" s="17"/>
       <c r="M230" s="17"/>
-      <c r="N230" s="17"/>
+      <c r="N230" s="17" t="s">
+        <v>75</v>
+      </c>
       <c r="O230" s="17"/>
-      <c r="P230" s="17"/>
+      <c r="P230" s="17" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="231" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B231" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C231" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D231" s="18" t="s">
-        <v>26</v>
+      <c r="A231" s="97" t="s">
+        <v>260</v>
+      </c>
+      <c r="B231" s="77" t="s">
+        <v>505</v>
+      </c>
+      <c r="C231" s="77" t="s">
+        <v>505</v>
+      </c>
+      <c r="D231" s="17">
+        <v>1</v>
       </c>
       <c r="E231" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F231" s="18"/>
-      <c r="G231" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="H231" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I231" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="J231" s="20"/>
-      <c r="K231" s="21"/>
+        <v>79</v>
+      </c>
+      <c r="F231" s="37" t="s">
+        <v>525</v>
+      </c>
+      <c r="G231" s="17"/>
+      <c r="H231" s="97" t="s">
+        <v>64</v>
+      </c>
+      <c r="I231" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="J231" s="73"/>
+      <c r="K231" s="74"/>
       <c r="L231" s="17"/>
       <c r="M231" s="17"/>
       <c r="N231" s="17" t="s">
@@ -11682,31 +11677,31 @@
       </c>
       <c r="O231" s="17"/>
       <c r="P231" s="17" t="s">
-        <v>257</v>
+        <v>75</v>
       </c>
     </row>
     <row r="232" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A232" s="97" t="s">
-        <v>260</v>
-      </c>
-      <c r="B232" s="77" t="s">
-        <v>505</v>
-      </c>
-      <c r="C232" s="77" t="s">
-        <v>505</v>
-      </c>
-      <c r="D232" s="17">
-        <v>1</v>
-      </c>
-      <c r="E232" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="F232" s="37" t="s">
-        <v>528</v>
-      </c>
-      <c r="G232" s="17"/>
-      <c r="H232" s="97" t="s">
-        <v>64</v>
+      <c r="A232" s="75" t="s">
+        <v>521</v>
+      </c>
+      <c r="B232" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="C232" s="79" t="s">
+        <v>523</v>
+      </c>
+      <c r="D232" s="78">
+        <v>1</v>
+      </c>
+      <c r="E232" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="F232" s="75"/>
+      <c r="G232" s="78">
+        <v>1</v>
+      </c>
+      <c r="H232" s="75" t="s">
+        <v>70</v>
       </c>
       <c r="I232" s="72" t="s">
         <v>29</v>
@@ -11720,31 +11715,31 @@
       </c>
       <c r="O232" s="17"/>
       <c r="P232" s="17" t="s">
-        <v>75</v>
+        <v>257</v>
       </c>
     </row>
     <row r="233" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="75" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="B233" s="76" t="s">
-        <v>525</v>
-      </c>
-      <c r="C233" s="79" t="s">
-        <v>526</v>
+        <v>529</v>
+      </c>
+      <c r="C233" s="76" t="s">
+        <v>530</v>
       </c>
       <c r="D233" s="78">
         <v>1</v>
       </c>
-      <c r="E233" s="75" t="s">
-        <v>66</v>
-      </c>
-      <c r="F233" s="75"/>
+      <c r="E233" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="F233" s="37"/>
       <c r="G233" s="78">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H233" s="75" t="s">
-        <v>70</v>
+        <v>515</v>
       </c>
       <c r="I233" s="72" t="s">
         <v>29</v>
@@ -11765,25 +11760,19 @@
       <c r="A234" s="75" t="s">
         <v>531</v>
       </c>
-      <c r="B234" s="76" t="s">
+      <c r="B234" s="76"/>
+      <c r="C234" s="76" t="s">
         <v>532</v>
       </c>
-      <c r="C234" s="76" t="s">
-        <v>533</v>
-      </c>
       <c r="D234" s="78">
         <v>1</v>
       </c>
       <c r="E234" s="89" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="F234" s="37"/>
-      <c r="G234" s="78">
-        <v>100</v>
-      </c>
-      <c r="H234" s="75" t="s">
-        <v>515</v>
-      </c>
+      <c r="G234" s="78"/>
+      <c r="H234" s="75"/>
       <c r="I234" s="72" t="s">
         <v>29</v>
       </c>
@@ -11800,97 +11789,105 @@
       </c>
     </row>
     <row r="235" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A235" s="75" t="s">
+      <c r="A235" s="116" t="s">
+        <v>533</v>
+      </c>
+      <c r="B235" s="117" t="s">
         <v>534</v>
       </c>
-      <c r="B235" s="76"/>
-      <c r="C235" s="76" t="s">
+      <c r="C235" s="103"/>
+      <c r="D235" s="104"/>
+      <c r="E235" s="105"/>
+      <c r="F235" s="105"/>
+      <c r="G235" s="104"/>
+      <c r="H235" s="105"/>
+      <c r="I235" s="105" t="s">
+        <v>277</v>
+      </c>
+      <c r="J235" s="105"/>
+      <c r="K235" s="106"/>
+      <c r="L235" s="107"/>
+      <c r="M235" s="102"/>
+      <c r="N235" s="102"/>
+      <c r="O235" s="102"/>
+      <c r="P235" s="102"/>
+    </row>
+    <row r="236" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B236" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="C236" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D236" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="E236" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="F236" s="67"/>
+      <c r="G236" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="H236" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="I236" s="108" t="s">
+        <v>29</v>
+      </c>
+      <c r="J236" s="109"/>
+      <c r="K236" s="110"/>
+      <c r="L236" s="102" t="s">
+        <v>493</v>
+      </c>
+      <c r="M236" s="111" t="s">
+        <v>183</v>
+      </c>
+      <c r="N236" s="102" t="s">
         <v>535</v>
       </c>
-      <c r="D235" s="78">
-        <v>1</v>
-      </c>
-      <c r="E235" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="F235" s="37"/>
-      <c r="G235" s="78"/>
-      <c r="H235" s="75"/>
-      <c r="I235" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="J235" s="73"/>
-      <c r="K235" s="74"/>
-      <c r="L235" s="17"/>
-      <c r="M235" s="17"/>
-      <c r="N235" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="O235" s="17"/>
-      <c r="P235" s="17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="236" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="133" t="s">
-        <v>536</v>
-      </c>
-      <c r="B236" s="134" t="s">
-        <v>537</v>
-      </c>
-      <c r="C236" s="120"/>
-      <c r="D236" s="121"/>
-      <c r="E236" s="122"/>
-      <c r="F236" s="122"/>
-      <c r="G236" s="121"/>
-      <c r="H236" s="122"/>
-      <c r="I236" s="122" t="s">
-        <v>277</v>
-      </c>
-      <c r="J236" s="122"/>
-      <c r="K236" s="123"/>
-      <c r="L236" s="124"/>
-      <c r="M236" s="102"/>
-      <c r="N236" s="102"/>
       <c r="O236" s="102"/>
-      <c r="P236" s="102"/>
+      <c r="P236" s="102" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="237" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A237" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="B237" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="C237" s="67" t="s">
-        <v>25</v>
-      </c>
-      <c r="D237" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="E237" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="F237" s="67"/>
-      <c r="G237" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="H237" s="67" t="s">
-        <v>28</v>
-      </c>
-      <c r="I237" s="125" t="s">
-        <v>29</v>
-      </c>
-      <c r="J237" s="126"/>
-      <c r="K237" s="127"/>
+      <c r="A237" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="B237" s="69" t="s">
+        <v>347</v>
+      </c>
+      <c r="C237" s="70" t="s">
+        <v>348</v>
+      </c>
+      <c r="D237" s="71">
+        <v>1</v>
+      </c>
+      <c r="E237" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="F237" s="68"/>
+      <c r="G237" s="71"/>
+      <c r="H237" s="68"/>
+      <c r="I237" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J237" s="113"/>
+      <c r="K237" s="114" t="s">
+        <v>29</v>
+      </c>
       <c r="L237" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M237" s="128" t="s">
+      <c r="M237" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N237" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O237" s="102"/>
       <c r="P237" s="102" t="s">
@@ -11898,39 +11895,41 @@
       </c>
     </row>
     <row r="238" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A238" s="68" t="s">
-        <v>346</v>
-      </c>
-      <c r="B238" s="69" t="s">
-        <v>347</v>
-      </c>
-      <c r="C238" s="70" t="s">
-        <v>348</v>
-      </c>
-      <c r="D238" s="71">
-        <v>1</v>
-      </c>
-      <c r="E238" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="F238" s="68"/>
-      <c r="G238" s="71"/>
-      <c r="H238" s="68"/>
-      <c r="I238" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J238" s="130"/>
-      <c r="K238" s="131" t="s">
+      <c r="A238" s="100" t="s">
+        <v>536</v>
+      </c>
+      <c r="B238" s="101" t="s">
+        <v>537</v>
+      </c>
+      <c r="C238" s="101" t="s">
+        <v>538</v>
+      </c>
+      <c r="D238" s="102">
+        <v>1</v>
+      </c>
+      <c r="E238" s="100" t="s">
+        <v>62</v>
+      </c>
+      <c r="F238" s="100"/>
+      <c r="G238" s="102"/>
+      <c r="H238" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="I238" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J238" s="113"/>
+      <c r="K238" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L238" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M238" s="128" t="s">
+      <c r="M238" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N238" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O238" s="102"/>
       <c r="P238" s="102" t="s">
@@ -11958,21 +11957,21 @@
       <c r="H239" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I239" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J239" s="130"/>
-      <c r="K239" s="132" t="s">
+      <c r="I239" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J239" s="113"/>
+      <c r="K239" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L239" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M239" s="128" t="s">
+      <c r="M239" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N239" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O239" s="102"/>
       <c r="P239" s="102" t="s">
@@ -12000,21 +11999,21 @@
       <c r="H240" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I240" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J240" s="130"/>
-      <c r="K240" s="132" t="s">
+      <c r="I240" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J240" s="113"/>
+      <c r="K240" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L240" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M240" s="128" t="s">
+      <c r="M240" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N240" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O240" s="102"/>
       <c r="P240" s="102" t="s">
@@ -12042,21 +12041,21 @@
       <c r="H241" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I241" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J241" s="130"/>
-      <c r="K241" s="132" t="s">
+      <c r="I241" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J241" s="113"/>
+      <c r="K241" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L241" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M241" s="128" t="s">
+      <c r="M241" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N241" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O241" s="102"/>
       <c r="P241" s="102" t="s">
@@ -12084,21 +12083,21 @@
       <c r="H242" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I242" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J242" s="130"/>
-      <c r="K242" s="132" t="s">
+      <c r="I242" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J242" s="113"/>
+      <c r="K242" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L242" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M242" s="128" t="s">
+      <c r="M242" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N242" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O242" s="102"/>
       <c r="P242" s="102" t="s">
@@ -12126,21 +12125,21 @@
       <c r="H243" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I243" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J243" s="130"/>
-      <c r="K243" s="132" t="s">
+      <c r="I243" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J243" s="113"/>
+      <c r="K243" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L243" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M243" s="128" t="s">
+      <c r="M243" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N243" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O243" s="102"/>
       <c r="P243" s="102" t="s">
@@ -12168,21 +12167,21 @@
       <c r="H244" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I244" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J244" s="130"/>
-      <c r="K244" s="132" t="s">
+      <c r="I244" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J244" s="113"/>
+      <c r="K244" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L244" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M244" s="128" t="s">
+      <c r="M244" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N244" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O244" s="102"/>
       <c r="P244" s="102" t="s">
@@ -12210,21 +12209,21 @@
       <c r="H245" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I245" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J245" s="130"/>
-      <c r="K245" s="132" t="s">
+      <c r="I245" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J245" s="113"/>
+      <c r="K245" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L245" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M245" s="128" t="s">
+      <c r="M245" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N245" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O245" s="102"/>
       <c r="P245" s="102" t="s">
@@ -12252,21 +12251,21 @@
       <c r="H246" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="I246" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J246" s="130"/>
-      <c r="K246" s="132" t="s">
+      <c r="I246" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="J246" s="113"/>
+      <c r="K246" s="115" t="s">
         <v>29</v>
       </c>
       <c r="L246" s="102" t="s">
         <v>493</v>
       </c>
-      <c r="M246" s="128" t="s">
+      <c r="M246" s="111" t="s">
         <v>183</v>
       </c>
       <c r="N246" s="102" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O246" s="102"/>
       <c r="P246" s="102" t="s">
@@ -12274,92 +12273,86 @@
       </c>
     </row>
     <row r="247" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A247" s="100" t="s">
+      <c r="A247" s="59" t="s">
         <v>563</v>
       </c>
-      <c r="B247" s="101" t="s">
+      <c r="B247" s="95" t="s">
         <v>564</v>
       </c>
-      <c r="C247" s="101" t="s">
-        <v>565</v>
-      </c>
-      <c r="D247" s="102">
-        <v>1</v>
-      </c>
-      <c r="E247" s="100" t="s">
-        <v>62</v>
-      </c>
-      <c r="F247" s="100"/>
-      <c r="G247" s="102"/>
-      <c r="H247" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="I247" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="J247" s="130"/>
-      <c r="K247" s="132" t="s">
-        <v>29</v>
-      </c>
-      <c r="L247" s="102" t="s">
-        <v>493</v>
-      </c>
-      <c r="M247" s="128" t="s">
-        <v>183</v>
-      </c>
-      <c r="N247" s="102" t="s">
-        <v>538</v>
-      </c>
-      <c r="O247" s="102"/>
-      <c r="P247" s="102" t="s">
-        <v>493</v>
-      </c>
+      <c r="C247" s="98"/>
+      <c r="D247" s="99"/>
+      <c r="E247" s="65"/>
+      <c r="F247" s="65"/>
+      <c r="G247" s="99"/>
+      <c r="H247" s="65"/>
+      <c r="I247" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="J247" s="65"/>
+      <c r="K247" s="66"/>
+      <c r="L247" s="17"/>
+      <c r="M247" s="17"/>
+      <c r="N247" s="17"/>
+      <c r="O247" s="17"/>
+      <c r="P247" s="17"/>
     </row>
     <row r="248" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A248" s="59" t="s">
-        <v>566</v>
-      </c>
-      <c r="B248" s="95" t="s">
-        <v>567</v>
-      </c>
-      <c r="C248" s="98"/>
-      <c r="D248" s="99"/>
-      <c r="E248" s="65"/>
-      <c r="F248" s="65"/>
-      <c r="G248" s="99"/>
-      <c r="H248" s="65"/>
-      <c r="I248" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="J248" s="65"/>
-      <c r="K248" s="66"/>
-      <c r="L248" s="17"/>
+      <c r="A248" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="B248" s="76" t="s">
+        <v>524</v>
+      </c>
+      <c r="C248" s="76" t="s">
+        <v>524</v>
+      </c>
+      <c r="D248" s="78">
+        <v>1</v>
+      </c>
+      <c r="E248" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="F248" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="G248" s="78"/>
+      <c r="H248" s="75"/>
+      <c r="I248" s="72" t="s">
+        <v>29</v>
+      </c>
+      <c r="J248" s="73"/>
+      <c r="K248" s="74"/>
+      <c r="L248" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="M248" s="17"/>
       <c r="N248" s="17"/>
       <c r="O248" s="17"/>
       <c r="P248" s="17"/>
     </row>
     <row r="249" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A249" s="75" t="s">
-        <v>476</v>
-      </c>
-      <c r="B249" s="76" t="s">
-        <v>527</v>
-      </c>
-      <c r="C249" s="76" t="s">
-        <v>527</v>
-      </c>
-      <c r="D249" s="78">
-        <v>1</v>
-      </c>
-      <c r="E249" s="89" t="s">
-        <v>79</v>
-      </c>
-      <c r="F249" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="G249" s="78"/>
-      <c r="H249" s="75"/>
+      <c r="A249" s="97" t="s">
+        <v>565</v>
+      </c>
+      <c r="B249" s="77" t="s">
+        <v>566</v>
+      </c>
+      <c r="C249" s="77" t="s">
+        <v>567</v>
+      </c>
+      <c r="D249" s="17">
+        <v>1</v>
+      </c>
+      <c r="E249" s="97" t="s">
+        <v>488</v>
+      </c>
+      <c r="F249" s="97"/>
+      <c r="G249" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="H249" s="97" t="s">
+        <v>493</v>
+      </c>
       <c r="I249" s="72" t="s">
         <v>29</v>
       </c>
@@ -12375,10 +12368,10 @@
     </row>
     <row r="250" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="97" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B250" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C250" s="77" t="s">
         <v>570</v>
@@ -12387,14 +12380,12 @@
         <v>1</v>
       </c>
       <c r="E250" s="97" t="s">
-        <v>488</v>
+        <v>62</v>
       </c>
       <c r="F250" s="97"/>
-      <c r="G250" s="17" t="s">
-        <v>571</v>
-      </c>
+      <c r="G250" s="17"/>
       <c r="H250" s="97" t="s">
-        <v>493</v>
+        <v>64</v>
       </c>
       <c r="I250" s="72" t="s">
         <v>29</v>
@@ -12411,13 +12402,13 @@
     </row>
     <row r="251" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="97" t="s">
+        <v>571</v>
+      </c>
+      <c r="B251" s="77" t="s">
+        <v>566</v>
+      </c>
+      <c r="C251" s="77" t="s">
         <v>572</v>
-      </c>
-      <c r="B251" s="77" t="s">
-        <v>569</v>
-      </c>
-      <c r="C251" s="77" t="s">
-        <v>573</v>
       </c>
       <c r="D251" s="17">
         <v>1</v>
@@ -12425,8 +12416,10 @@
       <c r="E251" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="F251" s="97"/>
-      <c r="G251" s="17"/>
+      <c r="F251" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="G251" s="57"/>
       <c r="H251" s="97" t="s">
         <v>64</v>
       </c>
@@ -12448,7 +12441,7 @@
         <v>574</v>
       </c>
       <c r="B252" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C252" s="77" t="s">
         <v>575</v>
@@ -12457,14 +12450,16 @@
         <v>1</v>
       </c>
       <c r="E252" s="97" t="s">
-        <v>62</v>
-      </c>
-      <c r="F252" s="17" t="s">
         <v>576</v>
       </c>
-      <c r="G252" s="57"/>
+      <c r="F252" s="97" t="s">
+        <v>577</v>
+      </c>
+      <c r="G252" s="17">
+        <v>10</v>
+      </c>
       <c r="H252" s="97" t="s">
-        <v>64</v>
+        <v>578</v>
       </c>
       <c r="I252" s="72" t="s">
         <v>29</v>
@@ -12481,26 +12476,22 @@
     </row>
     <row r="253" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="97" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="B253" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C253" s="77" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="D253" s="17">
         <v>1</v>
       </c>
       <c r="E253" s="97" t="s">
-        <v>579</v>
-      </c>
-      <c r="F253" s="97" t="s">
-        <v>580</v>
-      </c>
-      <c r="G253" s="17">
-        <v>10</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F253" s="97"/>
+      <c r="G253" s="17"/>
       <c r="H253" s="97" t="s">
         <v>581</v>
       </c>
@@ -12522,21 +12513,25 @@
         <v>582</v>
       </c>
       <c r="B254" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C254" s="77" t="s">
         <v>583</v>
       </c>
       <c r="D254" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E254" s="97" t="s">
-        <v>62</v>
-      </c>
-      <c r="F254" s="97"/>
-      <c r="G254" s="17"/>
+        <v>488</v>
+      </c>
+      <c r="F254" s="97" t="s">
+        <v>584</v>
+      </c>
+      <c r="G254" s="17">
+        <v>100</v>
+      </c>
       <c r="H254" s="97" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="I254" s="72" t="s">
         <v>29</v>
@@ -12553,28 +12548,28 @@
     </row>
     <row r="255" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="97" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B255" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C255" s="77" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D255" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E255" s="97" t="s">
         <v>488</v>
       </c>
       <c r="F255" s="97" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="G255" s="17">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H255" s="97" t="s">
-        <v>588</v>
+        <v>58</v>
       </c>
       <c r="I255" s="72" t="s">
         <v>29</v>
@@ -12594,7 +12589,7 @@
         <v>589</v>
       </c>
       <c r="B256" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C256" s="77" t="s">
         <v>590</v>
@@ -12603,16 +12598,14 @@
         <v>1</v>
       </c>
       <c r="E256" s="97" t="s">
-        <v>488</v>
+        <v>62</v>
       </c>
       <c r="F256" s="97" t="s">
         <v>591</v>
       </c>
-      <c r="G256" s="17">
-        <v>1000</v>
-      </c>
+      <c r="G256" s="17"/>
       <c r="H256" s="97" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="I256" s="72" t="s">
         <v>29</v>
@@ -12632,7 +12625,7 @@
         <v>592</v>
       </c>
       <c r="B257" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C257" s="77" t="s">
         <v>593</v>
@@ -12646,9 +12639,11 @@
       <c r="F257" s="97" t="s">
         <v>594</v>
       </c>
-      <c r="G257" s="17"/>
+      <c r="G257" s="17">
+        <v>10</v>
+      </c>
       <c r="H257" s="97" t="s">
-        <v>64</v>
+        <v>595</v>
       </c>
       <c r="I257" s="72" t="s">
         <v>29</v>
@@ -12665,13 +12660,13 @@
     </row>
     <row r="258" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="97" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B258" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C258" s="77" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D258" s="17">
         <v>1</v>
@@ -12680,13 +12675,13 @@
         <v>62</v>
       </c>
       <c r="F258" s="97" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G258" s="17">
         <v>10</v>
       </c>
       <c r="H258" s="97" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="I258" s="72" t="s">
         <v>29</v>
@@ -12703,13 +12698,13 @@
     </row>
     <row r="259" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="97" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B259" s="77" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C259" s="77" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D259" s="17">
         <v>1</v>
@@ -12718,13 +12713,13 @@
         <v>62</v>
       </c>
       <c r="F259" s="97" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="G259" s="17">
         <v>10</v>
       </c>
       <c r="H259" s="97" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="I259" s="72" t="s">
         <v>29</v>
@@ -12738,44 +12733,6 @@
       <c r="N259" s="17"/>
       <c r="O259" s="17"/>
       <c r="P259" s="17"/>
-    </row>
-    <row r="260" spans="1:16" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A260" s="97" t="s">
-        <v>600</v>
-      </c>
-      <c r="B260" s="77" t="s">
-        <v>569</v>
-      </c>
-      <c r="C260" s="77" t="s">
-        <v>596</v>
-      </c>
-      <c r="D260" s="17">
-        <v>1</v>
-      </c>
-      <c r="E260" s="97" t="s">
-        <v>62</v>
-      </c>
-      <c r="F260" s="97" t="s">
-        <v>597</v>
-      </c>
-      <c r="G260" s="17">
-        <v>10</v>
-      </c>
-      <c r="H260" s="97" t="s">
-        <v>598</v>
-      </c>
-      <c r="I260" s="72" t="s">
-        <v>29</v>
-      </c>
-      <c r="J260" s="73"/>
-      <c r="K260" s="74"/>
-      <c r="L260" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="M260" s="17"/>
-      <c r="N260" s="17"/>
-      <c r="O260" s="17"/>
-      <c r="P260" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>